<commit_message>
added code to (1) extract MINICOG/SLUMS/BNT/BVRT test results; (2) handle full note
</commit_message>
<xml_diff>
--- a/AD_cogtest_1.0/sample_for_cogtests.xlsx
+++ b/AD_cogtest_1.0/sample_for_cogtests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchen\Home\cjy\Research_2020_2029\projects\VA_Eisai\NLP_cogtest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchen\Home\cjy\Research_2020_2029\projects\VA_Eisai\NLP_cogtest\code\AD_cogtest_1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873C2EA9-2400-4151-89DF-EE12BC64708A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0C02F5-E278-428C-BEEF-AC0F89C82B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-86" yWindow="-86" windowWidth="14572" windowHeight="9172" xr2:uid="{913D1E7E-F989-4958-9BD3-2F105E5E2ED5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Montreal Cognitive Assement (MOCA): The total score (10/30) suggests...</t>
   </si>
@@ -80,43 +80,26 @@
     <t xml:space="preserve">MOCA: 25/30 (previous one was 23/30) </t>
   </si>
   <si>
-    <t>PHYSICIAN PROBLEM LIST:</t>
-  </si>
-  <si>
-    <t>B12 540</t>
-  </si>
-  <si>
-    <t>TSH 1.45</t>
-  </si>
-  <si>
-    <t>MRI: small vessel ischemic changes</t>
-  </si>
-  <si>
-    <t>REPEAT evaluation 11/2007: MMSE 24/30...</t>
-  </si>
-  <si>
-    <t>Mental Status Exam:</t>
-  </si>
-  <si>
-    <t>...</t>
-  </si>
-  <si>
-    <t>MMSE 25/30</t>
-  </si>
-  <si>
-    <t>MMSE 28/30 (October 2006 -- 1/3 spointaneous recall); clock drawing intact, 25/30 (June 2008)</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>NewOverallID</t>
-  </si>
-  <si>
     <t>ReportText</t>
   </si>
   <si>
     <t xml:space="preserve">MoCA               18 moderate impairment </t>
+  </si>
+  <si>
+    <t>NoteID</t>
+  </si>
+  <si>
+    <t>PHYSICIAN PROBLEM LIST:
+MMSE 28/30 (October 2006 -- 1/3 spointaneous recall); clock drawing intact, 25/30 (June 2008)
+B12 540
+TSH 1.45
+MRI: small vessel ischemic changes
+REPEAT evaluation 11/2007: MMSE 24/30...
+…
+Mental Status Exam:
+...
+MMSE 25/30
+…</t>
   </si>
 </sst>
 </file>
@@ -159,12 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3960C6-0C4D-42EC-A149-25C2F575335B}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="1"/>
@@ -493,10 +479,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.95" x14ac:dyDescent="1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.95" x14ac:dyDescent="1">
@@ -584,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.95" x14ac:dyDescent="1.05">
@@ -619,63 +605,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.95" x14ac:dyDescent="1">
+    <row r="17" spans="1:2" ht="191.25" x14ac:dyDescent="1">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B20" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B25" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B27" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
handle long integer NoteID; improving extraction strategies
</commit_message>
<xml_diff>
--- a/AD_cogtest_1.0/sample_for_cogtests.xlsx
+++ b/AD_cogtest_1.0/sample_for_cogtests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchen\Home\cjy\Research_2020_2029\projects\VA_Eisai\NLP_cogtest\code\AD_cogtest_1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0C02F5-E278-428C-BEEF-AC0F89C82B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852B7B28-F6DA-4BA9-AB9B-8382E4BDFA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-86" yWindow="-86" windowWidth="14572" windowHeight="9172" xr2:uid="{913D1E7E-F989-4958-9BD3-2F105E5E2ED5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Montreal Cognitive Assement (MOCA): The total score (10/30) suggests...</t>
   </si>
@@ -100,6 +100,15 @@
 ...
 MMSE 25/30
 …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mini-cog was performed on 11/09/2014 and the results were as follows: Recall: 0/3 Clock Drawing Test:  3/4 </t>
+  </si>
+  <si>
+    <t>..although he did well 26/30 on SLUMS. Loss of weight ~ 2 weeks 175 --&gt; 156 lbs...</t>
+  </si>
+  <si>
+    <t>...VS taken after SLUMS and GDS BS R 162/80, L 168/84…</t>
   </si>
 </sst>
 </file>
@@ -142,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -151,6 +160,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +478,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="1"/>
@@ -617,13 +627,25 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B19" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="1">
+      <c r="A19" s="4">
+        <v>1234567891012</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="15.95" x14ac:dyDescent="1">
-      <c r="B20" s="1"/>
+      <c r="A20">
+        <v>1234</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="15.95" x14ac:dyDescent="1">
       <c r="B21" s="1"/>

</xml_diff>